<commit_message>
Handled cases when a party is not in a poll
</commit_message>
<xml_diff>
--- a/fondamentaux/data/polls_1st_round/aggregated_polls.xlsx
+++ b/fondamentaux/data/polls_1st_round/aggregated_polls.xlsx
@@ -1,40 +1,87 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex_andorra/repos/pollsposition_models/fondamentaux/data/polls_1st_round/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8670BACE-16E9-9747-BD49-CC3B93CA5366}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19200" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>dateelection</t>
+  </si>
+  <si>
+    <t>samplesize_agg</t>
+  </si>
+  <si>
+    <t>farleft_agg</t>
+  </si>
+  <si>
+    <t>left_agg</t>
+  </si>
+  <si>
+    <t>green_agg</t>
+  </si>
+  <si>
+    <t>center_agg</t>
+  </si>
+  <si>
+    <t>right_agg</t>
+  </si>
+  <si>
+    <t>farright_agg</t>
+  </si>
+  <si>
+    <t>europeennes</t>
+  </si>
+  <si>
+    <t>regionales</t>
+  </si>
+  <si>
+    <t>legislatives</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt formatCode="yyyy-mm-dd h:mm:ss" numFmtId="164"/>
-    <numFmt formatCode="YYYY-MM-DD HH:MM:SS" numFmtId="165"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -49,27 +96,44 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="165" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -357,265 +421,231 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>dateelection</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>samplesize_agg</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>farleft_agg</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>left_agg</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>green_agg</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>center_agg</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>right_agg</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>farright_agg</t>
-        </is>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>europeennes</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2">
         <v>39971</v>
       </c>
-      <c r="D2" t="n">
+      <c r="D2">
         <v>2287</v>
       </c>
-      <c r="E2" t="n">
+      <c r="E2">
         <v>12.99453267007107</v>
       </c>
-      <c r="F2" t="n">
+      <c r="F2">
         <v>19.61478771495959</v>
       </c>
-      <c r="G2" t="n">
+      <c r="G2">
         <v>13.35153423532709</v>
       </c>
-      <c r="H2" t="n">
+      <c r="H2">
         <v>11.1684820808109</v>
       </c>
-      <c r="I2" t="n">
-        <v>27.26258673414158</v>
-      </c>
-      <c r="J2" t="n">
-        <v>5.756322266063732</v>
+      <c r="I2">
+        <v>27.262586734141578</v>
+      </c>
+      <c r="J2">
+        <v>5.7563222660637319</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
         <v>4</v>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>regionales</t>
-        </is>
-      </c>
-      <c r="C3" s="2" t="n">
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
         <v>40251</v>
       </c>
-      <c r="D3" t="n">
+      <c r="D3">
         <v>907</v>
       </c>
-      <c r="E3" t="n">
-        <v>9.827542768138009</v>
-      </c>
-      <c r="F3" t="n">
-        <v>28.9297161718842</v>
-      </c>
-      <c r="G3" t="n">
+      <c r="E3">
+        <v>9.8275427681380094</v>
+      </c>
+      <c r="F3">
+        <v>28.929716171884198</v>
+      </c>
+      <c r="G3">
         <v>13.58420361981117</v>
       </c>
-      <c r="H3" t="n">
-        <v>4.684000265532882</v>
-      </c>
-      <c r="I3" t="n">
-        <v>28.93073792740683</v>
-      </c>
-      <c r="J3" t="n">
-        <v>9.083516463389802</v>
+      <c r="H3">
+        <v>4.6840002655328821</v>
+      </c>
+      <c r="I3">
+        <v>28.930737927406831</v>
+      </c>
+      <c r="J3">
+        <v>9.0835164633898025</v>
       </c>
     </row>
-    <row r="4">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>legislatives</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2">
         <v>41070</v>
       </c>
-      <c r="D4" t="n">
+      <c r="D4">
         <v>1193</v>
       </c>
-      <c r="E4" t="n">
-        <v>7.973864868429566</v>
-      </c>
-      <c r="F4" t="n">
-        <v>32.11125265943151</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>2.775111578146919</v>
-      </c>
-      <c r="I4" t="n">
-        <v>33.68244436524814</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="E4">
+        <v>7.9738648684295663</v>
+      </c>
+      <c r="F4">
+        <v>32.111252659431507</v>
+      </c>
+      <c r="H4">
+        <v>2.7751115781469191</v>
+      </c>
+      <c r="I4">
+        <v>33.682444365248138</v>
+      </c>
+      <c r="J4">
         <v>15.25863568458217</v>
       </c>
     </row>
-    <row r="5">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>1</v>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>europeennes</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2">
         <v>41784</v>
       </c>
-      <c r="D5" t="n">
+      <c r="D5">
         <v>3248</v>
       </c>
-      <c r="E5" t="n">
-        <v>7.55630210443015</v>
-      </c>
-      <c r="F5" t="n">
-        <v>16.68915561513946</v>
-      </c>
-      <c r="G5" t="n">
-        <v>8.88391111731633</v>
-      </c>
-      <c r="H5" t="n">
-        <v>9.686673346084902</v>
-      </c>
-      <c r="I5" t="n">
-        <v>21.49759725516988</v>
-      </c>
-      <c r="J5" t="n">
-        <v>23.2142532792426</v>
+      <c r="E5">
+        <v>7.5563021044301504</v>
+      </c>
+      <c r="F5">
+        <v>16.689155615139459</v>
+      </c>
+      <c r="G5">
+        <v>8.8839111173163303</v>
+      </c>
+      <c r="H5">
+        <v>9.6866733460849019</v>
+      </c>
+      <c r="I5">
+        <v>21.497597255169879</v>
+      </c>
+      <c r="J5">
+        <v>23.214253279242602</v>
       </c>
     </row>
-    <row r="6">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>regionales</t>
-        </is>
-      </c>
-      <c r="C6" s="2" t="n">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
         <v>42344</v>
       </c>
-      <c r="D6" t="n">
+      <c r="D6">
         <v>1749</v>
       </c>
-      <c r="E6" t="n">
-        <v>5.267733514302111</v>
-      </c>
-      <c r="F6" t="n">
-        <v>22.90611009083124</v>
-      </c>
-      <c r="G6" t="n">
-        <v>5.860654376270849</v>
-      </c>
-      <c r="H6" t="inlineStr"/>
-      <c r="I6" t="n">
-        <v>28.11253252341348</v>
-      </c>
-      <c r="J6" t="n">
-        <v>28.88151680528222</v>
+      <c r="E6">
+        <v>5.2677335143021109</v>
+      </c>
+      <c r="F6">
+        <v>22.906110090831241</v>
+      </c>
+      <c r="G6">
+        <v>5.8606543762708494</v>
+      </c>
+      <c r="I6">
+        <v>28.112532523413481</v>
+      </c>
+      <c r="J6">
+        <v>28.881516805282221</v>
       </c>
     </row>
-    <row r="7">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>3</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>legislatives</t>
-        </is>
-      </c>
-      <c r="C7" s="2" t="n">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
         <v>42897</v>
       </c>
-      <c r="D7" t="n">
+      <c r="D7">
         <v>1299</v>
       </c>
-      <c r="E7" t="n">
+      <c r="E7">
         <v>11.70698665701012</v>
       </c>
-      <c r="F7" t="n">
-        <v>7.980058139295995</v>
-      </c>
-      <c r="G7" t="inlineStr"/>
-      <c r="H7" t="n">
-        <v>30.37535345478942</v>
-      </c>
-      <c r="I7" t="n">
-        <v>21.00566598781601</v>
-      </c>
-      <c r="J7" t="n">
+      <c r="F7">
+        <v>7.9800581392959948</v>
+      </c>
+      <c r="H7">
+        <v>30.375353454789419</v>
+      </c>
+      <c r="I7">
+        <v>21.005665987816009</v>
+      </c>
+      <c r="J7">
         <v>17.41608188288658</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>